<commit_message>
new file:   FanRenXiuXianIcon_1920_1080/hun_dun_ling_ta/tiao_zhan_over4.png 	new file:   FanRenXiuXianIcon_1920_1080/mo_dao_ru_qing/mo_dao_ru_qing_2.png 	modified:   bai_ye.py 	modified:   bai_zu_gong_feng.py 	modified:   boss_info.xlsx 	modified:   event_executor.py 	modified:   fu_ben.py 	modified:   game_control.py 	modified:   hong_bao.py 	modified:   hun_dun_ling_ta.py 	modified:   ling_shou.py 	modified:   lun_dao.py 	modified:   main.py 	modified:   mo_dao_ru_qing.py 	modified:   name_dict.py 	modified:   pa_tian_ti.py 	modified:   qi_xi_mo_jie.py 	modified:   shuang_xiu.py 	modified:   tiao_zhan_xian_yuan.py 	modified:   xiu_lian.py 	modified:   you_li.py 	modified:   zhui_mo_gu.py
</commit_message>
<xml_diff>
--- a/boss_info.xlsx
+++ b/boss_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\Projects\auto_xiuxian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630E0596-B62E-43E1-AA9B-56434BBE4AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E20634-343D-4780-9359-46DA6F822ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="231" yWindow="3600" windowWidth="22003" windowHeight="11914" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1791" yWindow="3334" windowWidth="20778" windowHeight="11915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="人界" sheetId="1" r:id="rId1"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1570,7 +1570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394BF15A-D4C5-4DBB-A35B-7EFBFC85100D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>

</xml_diff>